<commit_message>
colour change - web 2
</commit_message>
<xml_diff>
--- a/unit-1-sem-1/calendar-sem-1-2025.xlsx
+++ b/unit-1-sem-1/calendar-sem-1-2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fxwal\OneDrive\Desktop\repos\2024\hdip\2025\sem-1-calendar\unit-1-sem-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91963636-9EA1-4C29-A049-0034FBBE3F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB0B4F5-C68A-42DC-809C-C2F7378470AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11355" yWindow="-16395" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17445" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="option-2" sheetId="1" r:id="rId1"/>
@@ -722,12 +722,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="16"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="17"/>
         <bgColor auto="1"/>
       </patternFill>
@@ -789,6 +783,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1414,9 +1414,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1456,7 +1453,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1465,13 +1462,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1489,16 +1486,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="12" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="12" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="9" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
@@ -1510,13 +1507,13 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="11" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="10" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="16" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="16" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1537,16 +1534,16 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1555,13 +1552,13 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1576,7 +1573,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1591,57 +1588,75 @@
     <xf numFmtId="49" fontId="22" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="49" fontId="17" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="9" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="10" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="9" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="23" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1654,35 +1669,20 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="23" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2015,7 +2015,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-            <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
+            <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
           </a:ext>
         </a:extLst>
       </xdr:spPr>
@@ -2156,7 +2156,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-            <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
+            <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
           </a:ext>
         </a:extLst>
       </xdr:spPr>
@@ -3685,9 +3685,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K30"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:J30"/>
+      <selection pane="topRight" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.36328125" defaultRowHeight="20.25" customHeight="1"/>
@@ -3703,8 +3703,8 @@
   <sheetData>
     <row r="1" spans="2:11" ht="78.75" customHeight="1"/>
     <row r="2" spans="2:11" ht="25.75" customHeight="1">
-      <c r="B2" s="97"/>
-      <c r="C2" s="98"/>
+      <c r="B2" s="105"/>
+      <c r="C2" s="106"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -3715,8 +3715,8 @@
       <c r="K2" s="4"/>
     </row>
     <row r="3" spans="2:11" ht="23.25" customHeight="1">
-      <c r="B3" s="95"/>
-      <c r="C3" s="111"/>
+      <c r="B3" s="103"/>
+      <c r="C3" s="104"/>
       <c r="D3" s="5" t="s">
         <v>0</v>
       </c>
@@ -3971,7 +3971,7 @@
     </row>
     <row r="11" spans="2:11" ht="20" customHeight="1">
       <c r="B11" s="18"/>
-      <c r="C11" s="94" t="s">
+      <c r="C11" s="93" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="15">
@@ -4108,7 +4108,7 @@
     </row>
     <row r="15" spans="2:11" ht="20" customHeight="1">
       <c r="B15" s="30"/>
-      <c r="C15" s="94" t="s">
+      <c r="C15" s="93" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="15">
@@ -4420,10 +4420,10 @@
         <v>19</v>
       </c>
       <c r="F24" s="22">
-        <f t="shared" ref="F24:J24" si="22">E24+1</f>
+        <f t="shared" ref="F24:J28" si="22">E24+1</f>
         <v>20</v>
       </c>
-      <c r="G24" s="36">
+      <c r="G24" s="125">
         <f t="shared" si="22"/>
         <v>21</v>
       </c>
@@ -4457,8 +4457,8 @@
         <f t="shared" ref="F25:J25" si="23">E25+1</f>
         <v>27</v>
       </c>
-      <c r="G25" s="36">
-        <f t="shared" si="23"/>
+      <c r="G25" s="125">
+        <f t="shared" si="22"/>
         <v>28</v>
       </c>
       <c r="H25" s="16">
@@ -4493,8 +4493,8 @@
         <f t="shared" ref="F26:J26" si="24">E26+1</f>
         <v>3</v>
       </c>
-      <c r="G26" s="36">
-        <f t="shared" si="24"/>
+      <c r="G26" s="125">
+        <f t="shared" si="22"/>
         <v>4</v>
       </c>
       <c r="H26" s="22">
@@ -4509,7 +4509,7 @@
         <f t="shared" si="24"/>
         <v>7</v>
       </c>
-      <c r="K26" s="37"/>
+      <c r="K26" s="36"/>
     </row>
     <row r="27" spans="2:11" ht="20" customHeight="1">
       <c r="B27" s="30"/>
@@ -4527,8 +4527,8 @@
         <f t="shared" ref="F27:J27" si="25">E27+1</f>
         <v>10</v>
       </c>
-      <c r="G27" s="36">
-        <f t="shared" si="25"/>
+      <c r="G27" s="125">
+        <f t="shared" si="22"/>
         <v>11</v>
       </c>
       <c r="H27" s="16">
@@ -4553,7 +4553,7 @@
       <c r="D28" s="20">
         <v>15</v>
       </c>
-      <c r="E28" s="36">
+      <c r="E28" s="125">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
@@ -4561,8 +4561,8 @@
         <f t="shared" ref="F28:J28" si="26">E28+1</f>
         <v>17</v>
       </c>
-      <c r="G28" s="36">
-        <f t="shared" si="26"/>
+      <c r="G28" s="125">
+        <f t="shared" si="22"/>
         <v>18</v>
       </c>
       <c r="H28" s="22">
@@ -4577,7 +4577,7 @@
         <f t="shared" si="26"/>
         <v>21</v>
       </c>
-      <c r="K28" s="37"/>
+      <c r="K28" s="36"/>
     </row>
     <row r="29" spans="2:11" ht="20" customHeight="1">
       <c r="B29" s="18"/>
@@ -4612,35 +4612,35 @@
       <c r="K29" s="17"/>
     </row>
     <row r="30" spans="2:11" ht="19.75" customHeight="1">
-      <c r="B30" s="38"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="40">
+      <c r="B30" s="37"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="39">
         <v>29</v>
       </c>
-      <c r="E30" s="41">
+      <c r="E30" s="40">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="F30" s="41">
+      <c r="F30" s="40">
         <v>1</v>
       </c>
-      <c r="G30" s="41">
+      <c r="G30" s="40">
         <f t="shared" ref="G30:J30" si="28">F30+1</f>
         <v>2</v>
       </c>
-      <c r="H30" s="41">
+      <c r="H30" s="40">
         <f t="shared" si="28"/>
         <v>3</v>
       </c>
-      <c r="I30" s="41">
+      <c r="I30" s="40">
         <f t="shared" si="28"/>
         <v>4</v>
       </c>
-      <c r="J30" s="41">
+      <c r="J30" s="40">
         <f t="shared" si="28"/>
         <v>5</v>
       </c>
-      <c r="K30" s="42"/>
+      <c r="K30" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4678,8 +4678,8 @@
   <sheetData>
     <row r="1" spans="2:11" ht="78.75" customHeight="1"/>
     <row r="2" spans="2:11" ht="25.75" customHeight="1">
-      <c r="B2" s="97"/>
-      <c r="C2" s="98"/>
+      <c r="B2" s="105"/>
+      <c r="C2" s="106"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -4690,8 +4690,8 @@
       <c r="K2" s="4"/>
     </row>
     <row r="3" spans="2:11" ht="23.25" customHeight="1">
-      <c r="B3" s="95"/>
-      <c r="C3" s="96"/>
+      <c r="B3" s="103"/>
+      <c r="C3" s="107"/>
       <c r="D3" s="5" t="s">
         <v>0</v>
       </c>
@@ -4716,7 +4716,7 @@
       <c r="K3" s="7"/>
     </row>
     <row r="4" spans="2:11" ht="20.25" customHeight="1">
-      <c r="B4" s="43"/>
+      <c r="B4" s="42"/>
       <c r="C4" s="9" t="s">
         <v>5</v>
       </c>
@@ -4744,7 +4744,7 @@
       <c r="K4" s="12"/>
     </row>
     <row r="5" spans="2:11" ht="20" customHeight="1">
-      <c r="B5" s="44">
+      <c r="B5" s="43">
         <v>42005</v>
       </c>
       <c r="C5" s="14"/>
@@ -4856,10 +4856,10 @@
       <c r="K8" s="24"/>
     </row>
     <row r="9" spans="2:11" ht="20" customHeight="1">
-      <c r="B9" s="44">
+      <c r="B9" s="43">
         <v>42036</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="44" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="15">
@@ -4943,7 +4943,7 @@
     </row>
     <row r="12" spans="2:11" ht="20" customHeight="1">
       <c r="B12" s="33"/>
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="44" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="20">
@@ -4970,7 +4970,7 @@
       <c r="K12" s="24"/>
     </row>
     <row r="13" spans="2:11" ht="20" customHeight="1">
-      <c r="B13" s="44">
+      <c r="B13" s="43">
         <v>42064</v>
       </c>
       <c r="C13" s="34">
@@ -5001,7 +5001,7 @@
     </row>
     <row r="14" spans="2:11" ht="20" customHeight="1">
       <c r="B14" s="30"/>
-      <c r="C14" s="46">
+      <c r="C14" s="45">
         <v>7</v>
       </c>
       <c r="D14" s="20">
@@ -5029,7 +5029,7 @@
     </row>
     <row r="15" spans="2:11" ht="20" customHeight="1">
       <c r="B15" s="30"/>
-      <c r="C15" s="46">
+      <c r="C15" s="45">
         <v>8</v>
       </c>
       <c r="D15" s="15">
@@ -5057,7 +5057,7 @@
     </row>
     <row r="16" spans="2:11" ht="20" customHeight="1">
       <c r="B16" s="33"/>
-      <c r="C16" s="45" t="s">
+      <c r="C16" s="44" t="s">
         <v>7</v>
       </c>
       <c r="D16" s="20">
@@ -5084,10 +5084,10 @@
       <c r="K16" s="24"/>
     </row>
     <row r="17" spans="2:11" ht="20" customHeight="1">
-      <c r="B17" s="44">
+      <c r="B17" s="43">
         <v>42095</v>
       </c>
-      <c r="C17" s="47" t="s">
+      <c r="C17" s="46" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="15">
@@ -5115,7 +5115,7 @@
     </row>
     <row r="18" spans="2:11" ht="20" customHeight="1">
       <c r="B18" s="33"/>
-      <c r="C18" s="46">
+      <c r="C18" s="45">
         <v>9</v>
       </c>
       <c r="D18" s="20">
@@ -5143,7 +5143,7 @@
     </row>
     <row r="19" spans="2:11" ht="20" customHeight="1">
       <c r="B19" s="33"/>
-      <c r="C19" s="46">
+      <c r="C19" s="45">
         <v>10</v>
       </c>
       <c r="D19" s="15">
@@ -5198,7 +5198,7 @@
       <c r="K20" s="24"/>
     </row>
     <row r="21" spans="2:11" ht="20" customHeight="1">
-      <c r="B21" s="44">
+      <c r="B21" s="43">
         <v>42125</v>
       </c>
       <c r="C21" s="34">
@@ -5229,7 +5229,7 @@
     </row>
     <row r="22" spans="2:11" ht="20" customHeight="1">
       <c r="B22" s="30"/>
-      <c r="C22" s="48"/>
+      <c r="C22" s="47"/>
       <c r="D22" s="20">
         <v>5</v>
       </c>
@@ -5255,7 +5255,7 @@
     </row>
     <row r="23" spans="2:11" ht="20" customHeight="1">
       <c r="B23" s="30"/>
-      <c r="C23" s="49"/>
+      <c r="C23" s="48"/>
       <c r="D23" s="15">
         <v>12</v>
       </c>
@@ -5281,7 +5281,7 @@
     </row>
     <row r="24" spans="2:11" ht="20" customHeight="1">
       <c r="B24" s="33"/>
-      <c r="C24" s="46">
+      <c r="C24" s="45">
         <v>13</v>
       </c>
       <c r="D24" s="20">
@@ -5293,7 +5293,7 @@
       <c r="F24" s="22">
         <v>21</v>
       </c>
-      <c r="G24" s="50">
+      <c r="G24" s="49">
         <v>22</v>
       </c>
       <c r="H24" s="22">
@@ -5321,7 +5321,7 @@
       <c r="F25" s="16">
         <v>28</v>
       </c>
-      <c r="G25" s="50">
+      <c r="G25" s="49">
         <v>29</v>
       </c>
       <c r="H25" s="16">
@@ -5336,7 +5336,7 @@
       <c r="K25" s="17"/>
     </row>
     <row r="26" spans="2:11" ht="20" customHeight="1">
-      <c r="B26" s="44">
+      <c r="B26" s="43">
         <v>42156</v>
       </c>
       <c r="C26" s="19">
@@ -5351,7 +5351,7 @@
       <c r="F26" s="22">
         <v>4</v>
       </c>
-      <c r="G26" s="50">
+      <c r="G26" s="49">
         <v>5</v>
       </c>
       <c r="H26" s="22">
@@ -5363,7 +5363,7 @@
       <c r="J26" s="22">
         <v>8</v>
       </c>
-      <c r="K26" s="37"/>
+      <c r="K26" s="36"/>
     </row>
     <row r="27" spans="2:11" ht="20" customHeight="1">
       <c r="B27" s="30"/>
@@ -5379,7 +5379,7 @@
       <c r="F27" s="16">
         <v>11</v>
       </c>
-      <c r="G27" s="50">
+      <c r="G27" s="49">
         <v>12</v>
       </c>
       <c r="H27" s="16">
@@ -5401,13 +5401,13 @@
       <c r="D28" s="20">
         <v>16</v>
       </c>
-      <c r="E28" s="50">
+      <c r="E28" s="49">
         <v>17</v>
       </c>
       <c r="F28" s="22">
         <v>18</v>
       </c>
-      <c r="G28" s="50">
+      <c r="G28" s="49">
         <v>19</v>
       </c>
       <c r="H28" s="22">
@@ -5419,7 +5419,7 @@
       <c r="J28" s="22">
         <v>22</v>
       </c>
-      <c r="K28" s="37"/>
+      <c r="K28" s="36"/>
     </row>
     <row r="29" spans="2:11" ht="20" customHeight="1">
       <c r="B29" s="33"/>
@@ -5448,32 +5448,32 @@
       <c r="K29" s="17"/>
     </row>
     <row r="30" spans="2:11" ht="19.75" customHeight="1">
-      <c r="B30" s="51">
+      <c r="B30" s="50">
         <v>43647</v>
       </c>
-      <c r="C30" s="39"/>
-      <c r="D30" s="40">
+      <c r="C30" s="38"/>
+      <c r="D30" s="39">
         <v>30</v>
       </c>
-      <c r="E30" s="41">
+      <c r="E30" s="40">
         <v>1</v>
       </c>
-      <c r="F30" s="41">
+      <c r="F30" s="40">
         <v>2</v>
       </c>
-      <c r="G30" s="41">
+      <c r="G30" s="40">
         <v>3</v>
       </c>
-      <c r="H30" s="41">
+      <c r="H30" s="40">
         <v>4</v>
       </c>
-      <c r="I30" s="41">
+      <c r="I30" s="40">
         <v>5</v>
       </c>
-      <c r="J30" s="41">
+      <c r="J30" s="40">
         <v>6</v>
       </c>
-      <c r="K30" s="42"/>
+      <c r="K30" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5497,220 +5497,225 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.36328125" defaultRowHeight="20" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4.81640625" style="52" customWidth="1"/>
-    <col min="2" max="2" width="6.1796875" style="52" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" style="52" customWidth="1"/>
-    <col min="4" max="4" width="23.6328125" style="52" customWidth="1"/>
-    <col min="5" max="5" width="22.81640625" style="52" customWidth="1"/>
-    <col min="6" max="6" width="26.1796875" style="52" customWidth="1"/>
-    <col min="7" max="7" width="16.36328125" style="52" customWidth="1"/>
-    <col min="8" max="16384" width="16.36328125" style="52"/>
+    <col min="1" max="1" width="4.81640625" style="51" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" style="51" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="51" customWidth="1"/>
+    <col min="4" max="4" width="23.6328125" style="51" customWidth="1"/>
+    <col min="5" max="5" width="22.81640625" style="51" customWidth="1"/>
+    <col min="6" max="6" width="26.1796875" style="51" customWidth="1"/>
+    <col min="7" max="7" width="16.36328125" style="51" customWidth="1"/>
+    <col min="8" max="16384" width="16.36328125" style="51"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="14" customHeight="1"/>
     <row r="2" spans="2:6" ht="27.75" customHeight="1">
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="116" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
     </row>
     <row r="3" spans="2:6" ht="20" customHeight="1">
-      <c r="B3" s="53"/>
-      <c r="C3" s="54" t="s">
+      <c r="B3" s="52"/>
+      <c r="C3" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="55" t="s">
+      <c r="D3" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="55" t="s">
+      <c r="F3" s="54" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="30" customHeight="1">
-      <c r="B4" s="56"/>
-      <c r="C4" s="57">
+      <c r="B4" s="55"/>
+      <c r="C4" s="56">
         <v>44839.375</v>
       </c>
-      <c r="D4" s="100" t="s">
+      <c r="D4" s="110" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="101"/>
-      <c r="F4" s="58" t="s">
+      <c r="E4" s="112"/>
+      <c r="F4" s="57" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="60" customHeight="1">
-      <c r="B5" s="59"/>
-      <c r="C5" s="57">
+      <c r="B5" s="58"/>
+      <c r="C5" s="56">
         <v>44839.385416666664</v>
       </c>
-      <c r="D5" s="100" t="s">
+      <c r="D5" s="110" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="101"/>
-      <c r="F5" s="60"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="59"/>
     </row>
     <row r="6" spans="2:6" ht="30" customHeight="1">
-      <c r="B6" s="59"/>
-      <c r="C6" s="57">
+      <c r="B6" s="58"/>
+      <c r="C6" s="56">
         <v>44839.40625</v>
       </c>
-      <c r="D6" s="100" t="s">
+      <c r="D6" s="110" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="101"/>
-      <c r="F6" s="60"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="59"/>
     </row>
     <row r="7" spans="2:6" ht="35.25" customHeight="1">
-      <c r="B7" s="61"/>
-      <c r="C7" s="62">
+      <c r="B7" s="60"/>
+      <c r="C7" s="61">
         <v>44839.416666666664</v>
       </c>
-      <c r="D7" s="102" t="s">
+      <c r="D7" s="114" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="101"/>
-      <c r="F7" s="60"/>
+      <c r="E7" s="112"/>
+      <c r="F7" s="59"/>
     </row>
     <row r="8" spans="2:6" ht="60" customHeight="1">
-      <c r="B8" s="63"/>
-      <c r="C8" s="57">
+      <c r="B8" s="62"/>
+      <c r="C8" s="56">
         <v>44839.4375</v>
       </c>
-      <c r="D8" s="64" t="s">
+      <c r="D8" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="105" t="s">
+      <c r="E8" s="111" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="65" t="s">
+      <c r="F8" s="64" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="60" customHeight="1">
-      <c r="B9" s="59"/>
-      <c r="C9" s="57">
+      <c r="B9" s="58"/>
+      <c r="C9" s="56">
         <v>44839.458333333336</v>
       </c>
-      <c r="D9" s="64" t="s">
+      <c r="D9" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="101"/>
-      <c r="F9" s="60"/>
+      <c r="E9" s="112"/>
+      <c r="F9" s="59"/>
     </row>
     <row r="10" spans="2:6" ht="60" customHeight="1">
-      <c r="B10" s="59"/>
-      <c r="C10" s="57">
+      <c r="B10" s="58"/>
+      <c r="C10" s="56">
         <v>44839.479166666664</v>
       </c>
-      <c r="D10" s="106" t="s">
+      <c r="D10" s="113" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="105" t="s">
+      <c r="E10" s="111" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="65" t="s">
+      <c r="F10" s="64" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="60" customHeight="1">
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="104"/>
-      <c r="E11" s="101"/>
-      <c r="F11" s="60"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="109"/>
+      <c r="E11" s="112"/>
+      <c r="F11" s="59"/>
     </row>
     <row r="12" spans="2:6" ht="60" customHeight="1">
-      <c r="B12" s="59"/>
-      <c r="C12" s="66">
+      <c r="B12" s="58"/>
+      <c r="C12" s="65">
         <v>44839.520833333336</v>
       </c>
-      <c r="D12" s="100" t="s">
+      <c r="D12" s="110" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="101"/>
-      <c r="F12" s="67"/>
+      <c r="E12" s="112"/>
+      <c r="F12" s="66"/>
     </row>
     <row r="13" spans="2:6" ht="120" customHeight="1">
-      <c r="B13" s="61"/>
-      <c r="C13" s="62">
+      <c r="B13" s="60"/>
+      <c r="C13" s="61">
         <v>44839.541666666664</v>
       </c>
-      <c r="D13" s="102" t="s">
+      <c r="D13" s="114" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="104"/>
-      <c r="F13" s="107"/>
+      <c r="E13" s="109"/>
+      <c r="F13" s="115"/>
     </row>
     <row r="14" spans="2:6" ht="60" customHeight="1">
-      <c r="B14" s="59"/>
-      <c r="C14" s="57">
+      <c r="B14" s="58"/>
+      <c r="C14" s="56">
         <v>44839.583333333336</v>
       </c>
-      <c r="D14" s="100" t="s">
+      <c r="D14" s="110" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="104"/>
-      <c r="F14" s="68" t="s">
+      <c r="E14" s="109"/>
+      <c r="F14" s="67" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="60" customHeight="1">
-      <c r="B15" s="59"/>
-      <c r="C15" s="57">
+      <c r="B15" s="58"/>
+      <c r="C15" s="56">
         <v>44839.604166666664</v>
       </c>
-      <c r="D15" s="100" t="s">
+      <c r="D15" s="110" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="104"/>
-      <c r="F15" s="68" t="s">
+      <c r="E15" s="109"/>
+      <c r="F15" s="67" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="60" customHeight="1">
-      <c r="B16" s="69"/>
-      <c r="C16" s="62">
+      <c r="B16" s="68"/>
+      <c r="C16" s="61">
         <v>44839.625</v>
       </c>
-      <c r="D16" s="102" t="s">
+      <c r="D16" s="114" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="104"/>
-      <c r="F16" s="104"/>
+      <c r="E16" s="109"/>
+      <c r="F16" s="109"/>
     </row>
     <row r="17" spans="2:6" ht="120" customHeight="1">
-      <c r="B17" s="59"/>
-      <c r="C17" s="57">
+      <c r="B17" s="58"/>
+      <c r="C17" s="56">
         <v>44839.645833333336</v>
       </c>
-      <c r="D17" s="100" t="s">
+      <c r="D17" s="110" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="104"/>
-      <c r="F17" s="68" t="s">
+      <c r="E17" s="109"/>
+      <c r="F17" s="67" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="41" customHeight="1">
-      <c r="B18" s="69"/>
-      <c r="C18" s="70">
+      <c r="B18" s="68"/>
+      <c r="C18" s="69">
         <v>44839.708333333336</v>
       </c>
-      <c r="D18" s="103" t="s">
+      <c r="D18" s="108" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="104"/>
-      <c r="F18" s="104"/>
+      <c r="E18" s="109"/>
+      <c r="F18" s="109"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D4:E4"/>
     <mergeCell ref="D18:F18"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
@@ -5721,11 +5726,6 @@
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="D16:F16"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D4:E4"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup scale="70" orientation="portrait"/>
@@ -5742,813 +5742,819 @@
   </sheetPr>
   <dimension ref="A1:AN17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection sqref="A1:AN16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.36328125" defaultRowHeight="18" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" style="71" customWidth="1"/>
-    <col min="2" max="6" width="4.1796875" style="71" customWidth="1"/>
-    <col min="7" max="7" width="1.6328125" style="71" customWidth="1"/>
-    <col min="8" max="8" width="4.1796875" style="71" customWidth="1"/>
-    <col min="9" max="9" width="1.6328125" style="71" customWidth="1"/>
-    <col min="10" max="12" width="4.1796875" style="71" customWidth="1"/>
-    <col min="13" max="13" width="1.6328125" style="71" customWidth="1"/>
-    <col min="14" max="14" width="4.1796875" style="71" customWidth="1"/>
-    <col min="15" max="15" width="1.6328125" style="71" customWidth="1"/>
-    <col min="16" max="18" width="4.1796875" style="71" customWidth="1"/>
-    <col min="19" max="19" width="1.6328125" style="71" customWidth="1"/>
-    <col min="20" max="21" width="4.1796875" style="71" customWidth="1"/>
-    <col min="22" max="22" width="1.6328125" style="71" customWidth="1"/>
-    <col min="23" max="24" width="4.1796875" style="71" customWidth="1"/>
-    <col min="25" max="25" width="2.1796875" style="71" customWidth="1"/>
-    <col min="26" max="27" width="4.1796875" style="71" customWidth="1"/>
-    <col min="28" max="29" width="1.6328125" style="71" customWidth="1"/>
-    <col min="30" max="35" width="4.1796875" style="71" customWidth="1"/>
-    <col min="36" max="37" width="3.453125" style="71" customWidth="1"/>
-    <col min="38" max="38" width="11.6328125" style="71" customWidth="1"/>
-    <col min="39" max="39" width="2.6328125" style="71" customWidth="1"/>
-    <col min="40" max="40" width="12.1796875" style="71" customWidth="1"/>
-    <col min="41" max="41" width="16.36328125" style="71" customWidth="1"/>
-    <col min="42" max="16384" width="16.36328125" style="71"/>
+    <col min="1" max="1" width="17.81640625" style="70" customWidth="1"/>
+    <col min="2" max="6" width="4.1796875" style="70" customWidth="1"/>
+    <col min="7" max="7" width="1.6328125" style="70" customWidth="1"/>
+    <col min="8" max="8" width="4.1796875" style="70" customWidth="1"/>
+    <col min="9" max="9" width="1.6328125" style="70" customWidth="1"/>
+    <col min="10" max="12" width="4.1796875" style="70" customWidth="1"/>
+    <col min="13" max="13" width="1.6328125" style="70" customWidth="1"/>
+    <col min="14" max="14" width="4.1796875" style="70" customWidth="1"/>
+    <col min="15" max="15" width="1.6328125" style="70" customWidth="1"/>
+    <col min="16" max="18" width="4.1796875" style="70" customWidth="1"/>
+    <col min="19" max="19" width="1.6328125" style="70" customWidth="1"/>
+    <col min="20" max="21" width="4.1796875" style="70" customWidth="1"/>
+    <col min="22" max="22" width="1.6328125" style="70" customWidth="1"/>
+    <col min="23" max="24" width="4.1796875" style="70" customWidth="1"/>
+    <col min="25" max="25" width="2.1796875" style="70" customWidth="1"/>
+    <col min="26" max="27" width="4.1796875" style="70" customWidth="1"/>
+    <col min="28" max="29" width="1.6328125" style="70" customWidth="1"/>
+    <col min="30" max="35" width="4.1796875" style="70" customWidth="1"/>
+    <col min="36" max="37" width="3.453125" style="70" customWidth="1"/>
+    <col min="38" max="38" width="11.6328125" style="70" customWidth="1"/>
+    <col min="39" max="39" width="2.6328125" style="70" customWidth="1"/>
+    <col min="40" max="40" width="12.1796875" style="70" customWidth="1"/>
+    <col min="41" max="41" width="16.36328125" style="70" customWidth="1"/>
+    <col min="42" max="16384" width="16.36328125" style="70"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="20" customHeight="1">
-      <c r="A1" s="72"/>
-      <c r="B1" s="73"/>
-      <c r="C1" s="112">
+      <c r="A1" s="71"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="117">
         <v>43101</v>
       </c>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112">
+      <c r="D1" s="117"/>
+      <c r="E1" s="117">
         <v>43132</v>
       </c>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="112"/>
-      <c r="J1" s="112"/>
-      <c r="K1" s="113" t="s">
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
+      <c r="I1" s="117"/>
+      <c r="J1" s="117"/>
+      <c r="K1" s="118" t="s">
         <v>55</v>
       </c>
-      <c r="L1" s="114"/>
-      <c r="M1" s="114"/>
-      <c r="N1" s="114"/>
-      <c r="O1" s="114"/>
-      <c r="P1" s="114"/>
-      <c r="Q1" s="112">
+      <c r="L1" s="119"/>
+      <c r="M1" s="119"/>
+      <c r="N1" s="119"/>
+      <c r="O1" s="119"/>
+      <c r="P1" s="119"/>
+      <c r="Q1" s="117">
         <v>43191</v>
       </c>
-      <c r="R1" s="115"/>
-      <c r="S1" s="115"/>
-      <c r="T1" s="115"/>
-      <c r="U1" s="115"/>
-      <c r="V1" s="116"/>
-      <c r="W1" s="112">
+      <c r="R1" s="120"/>
+      <c r="S1" s="120"/>
+      <c r="T1" s="120"/>
+      <c r="U1" s="120"/>
+      <c r="V1" s="95"/>
+      <c r="W1" s="117">
         <v>43221</v>
       </c>
-      <c r="X1" s="115"/>
-      <c r="Y1" s="115"/>
-      <c r="Z1" s="115"/>
-      <c r="AA1" s="116"/>
-      <c r="AB1" s="117"/>
-      <c r="AC1" s="117"/>
-      <c r="AD1" s="112">
+      <c r="X1" s="120"/>
+      <c r="Y1" s="120"/>
+      <c r="Z1" s="120"/>
+      <c r="AA1" s="95"/>
+      <c r="AB1" s="94"/>
+      <c r="AC1" s="94"/>
+      <c r="AD1" s="117">
         <v>43983</v>
       </c>
-      <c r="AE1" s="115"/>
-      <c r="AF1" s="115"/>
-      <c r="AG1" s="115"/>
-      <c r="AH1" s="117"/>
-      <c r="AI1" s="117"/>
-      <c r="AJ1" s="117"/>
-      <c r="AK1" s="117"/>
-      <c r="AL1" s="118" t="s">
+      <c r="AE1" s="120"/>
+      <c r="AF1" s="120"/>
+      <c r="AG1" s="120"/>
+      <c r="AH1" s="94"/>
+      <c r="AI1" s="94"/>
+      <c r="AJ1" s="94"/>
+      <c r="AK1" s="94"/>
+      <c r="AL1" s="96" t="s">
         <v>35</v>
       </c>
-      <c r="AM1" s="112">
+      <c r="AM1" s="117">
         <v>43344</v>
       </c>
-      <c r="AN1" s="115"/>
+      <c r="AN1" s="120"/>
     </row>
     <row r="2" spans="1:40" ht="20" customHeight="1">
-      <c r="A2" s="119" t="s">
+      <c r="A2" s="97" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="123">
+      <c r="B2" s="71"/>
+      <c r="C2" s="101">
         <v>1</v>
       </c>
-      <c r="D2" s="123">
+      <c r="D2" s="101">
         <v>2</v>
       </c>
-      <c r="E2" s="123">
+      <c r="E2" s="101">
         <v>3</v>
       </c>
-      <c r="F2" s="123">
+      <c r="F2" s="101">
         <v>4</v>
       </c>
-      <c r="G2" s="117"/>
-      <c r="H2" s="124" t="s">
+      <c r="G2" s="94"/>
+      <c r="H2" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="117"/>
-      <c r="J2" s="123">
+      <c r="I2" s="94"/>
+      <c r="J2" s="101">
         <v>5</v>
       </c>
-      <c r="K2" s="123">
+      <c r="K2" s="101">
         <v>6</v>
       </c>
-      <c r="L2" s="123">
+      <c r="L2" s="101">
         <v>7</v>
       </c>
-      <c r="M2" s="117"/>
-      <c r="N2" s="124" t="s">
+      <c r="M2" s="94"/>
+      <c r="N2" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="O2" s="117"/>
-      <c r="P2" s="123">
+      <c r="O2" s="94"/>
+      <c r="P2" s="101">
         <v>6</v>
       </c>
-      <c r="Q2" s="123">
+      <c r="Q2" s="101">
         <v>7</v>
       </c>
-      <c r="R2" s="123">
+      <c r="R2" s="101">
         <v>8</v>
       </c>
-      <c r="S2" s="117"/>
-      <c r="T2" s="125" t="s">
+      <c r="S2" s="94"/>
+      <c r="T2" s="121" t="s">
         <v>38</v>
       </c>
-      <c r="U2" s="115"/>
-      <c r="V2" s="117"/>
-      <c r="W2" s="123">
+      <c r="U2" s="120"/>
+      <c r="V2" s="94"/>
+      <c r="W2" s="101">
         <v>11</v>
       </c>
-      <c r="X2" s="123">
+      <c r="X2" s="101">
         <v>12</v>
       </c>
-      <c r="Y2" s="116"/>
-      <c r="Z2" s="125" t="s">
+      <c r="Y2" s="95"/>
+      <c r="Z2" s="121" t="s">
         <v>37</v>
       </c>
-      <c r="AA2" s="115"/>
-      <c r="AB2" s="120"/>
-      <c r="AC2" s="117"/>
-      <c r="AD2" s="123">
+      <c r="AA2" s="120"/>
+      <c r="AB2" s="98"/>
+      <c r="AC2" s="94"/>
+      <c r="AD2" s="101">
         <v>13</v>
       </c>
-      <c r="AE2" s="123">
+      <c r="AE2" s="101">
         <v>14</v>
       </c>
-      <c r="AF2" s="123">
+      <c r="AF2" s="101">
         <v>15</v>
       </c>
-      <c r="AG2" s="123">
+      <c r="AG2" s="101">
         <v>16</v>
       </c>
-      <c r="AH2" s="123">
+      <c r="AH2" s="101">
         <v>17</v>
       </c>
-      <c r="AI2" s="123">
+      <c r="AI2" s="101">
         <v>18</v>
       </c>
-      <c r="AJ2" s="73"/>
-      <c r="AK2" s="73"/>
-      <c r="AL2" s="73"/>
-      <c r="AM2" s="73"/>
-      <c r="AN2" s="73"/>
+      <c r="AJ2" s="72"/>
+      <c r="AK2" s="72"/>
+      <c r="AL2" s="72"/>
+      <c r="AM2" s="72"/>
+      <c r="AN2" s="72"/>
     </row>
     <row r="3" spans="1:40" ht="10" customHeight="1">
-      <c r="A3" s="120"/>
-      <c r="B3" s="72"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-      <c r="L3" s="75"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="75"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="75"/>
-      <c r="Q3" s="75"/>
-      <c r="R3" s="75"/>
-      <c r="S3" s="72"/>
-      <c r="T3" s="75"/>
-      <c r="U3" s="75"/>
-      <c r="V3" s="72"/>
-      <c r="W3" s="75"/>
-      <c r="X3" s="75"/>
-      <c r="Y3" s="72"/>
-      <c r="Z3" s="75"/>
-      <c r="AA3" s="75"/>
-      <c r="AB3" s="74"/>
-      <c r="AC3" s="72"/>
-      <c r="AD3" s="72"/>
-      <c r="AE3" s="72"/>
-      <c r="AF3" s="72"/>
-      <c r="AG3" s="72"/>
-      <c r="AH3" s="72"/>
-      <c r="AI3" s="72"/>
-      <c r="AJ3" s="72"/>
-      <c r="AK3" s="72"/>
-      <c r="AL3" s="72"/>
-      <c r="AM3" s="72"/>
-      <c r="AN3" s="72"/>
+      <c r="A3" s="98"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="71"/>
+      <c r="N3" s="74"/>
+      <c r="O3" s="71"/>
+      <c r="P3" s="74"/>
+      <c r="Q3" s="74"/>
+      <c r="R3" s="74"/>
+      <c r="S3" s="71"/>
+      <c r="T3" s="74"/>
+      <c r="U3" s="74"/>
+      <c r="V3" s="71"/>
+      <c r="W3" s="74"/>
+      <c r="X3" s="74"/>
+      <c r="Y3" s="71"/>
+      <c r="Z3" s="74"/>
+      <c r="AA3" s="74"/>
+      <c r="AB3" s="73"/>
+      <c r="AC3" s="71"/>
+      <c r="AD3" s="71"/>
+      <c r="AE3" s="71"/>
+      <c r="AF3" s="71"/>
+      <c r="AG3" s="71"/>
+      <c r="AH3" s="71"/>
+      <c r="AI3" s="71"/>
+      <c r="AJ3" s="71"/>
+      <c r="AK3" s="71"/>
+      <c r="AL3" s="71"/>
+      <c r="AM3" s="71"/>
+      <c r="AN3" s="71"/>
     </row>
     <row r="4" spans="1:40" ht="35" customHeight="1">
-      <c r="A4" s="119" t="s">
+      <c r="A4" s="97" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="77"/>
-      <c r="K4" s="77"/>
-      <c r="L4" s="77"/>
-      <c r="M4" s="78"/>
-      <c r="N4" s="79"/>
-      <c r="O4" s="78"/>
-      <c r="P4" s="77"/>
-      <c r="Q4" s="77"/>
-      <c r="R4" s="77"/>
-      <c r="S4" s="78"/>
-      <c r="T4" s="79"/>
-      <c r="U4" s="79"/>
-      <c r="V4" s="78"/>
-      <c r="W4" s="77"/>
-      <c r="X4" s="77"/>
-      <c r="Y4" s="80"/>
-      <c r="Z4" s="79"/>
-      <c r="AA4" s="79"/>
-      <c r="AB4" s="81"/>
-      <c r="AC4" s="72"/>
-      <c r="AD4" s="72"/>
-      <c r="AE4" s="72"/>
-      <c r="AF4" s="72"/>
-      <c r="AG4" s="72"/>
-      <c r="AH4" s="72"/>
-      <c r="AI4" s="72"/>
-      <c r="AJ4" s="72"/>
-      <c r="AK4" s="72"/>
-      <c r="AL4" s="72"/>
-      <c r="AM4" s="72"/>
-      <c r="AN4" s="72"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
+      <c r="L4" s="76"/>
+      <c r="M4" s="77"/>
+      <c r="N4" s="78"/>
+      <c r="O4" s="77"/>
+      <c r="P4" s="76"/>
+      <c r="Q4" s="76"/>
+      <c r="R4" s="76"/>
+      <c r="S4" s="77"/>
+      <c r="T4" s="78"/>
+      <c r="U4" s="78"/>
+      <c r="V4" s="77"/>
+      <c r="W4" s="76"/>
+      <c r="X4" s="76"/>
+      <c r="Y4" s="79"/>
+      <c r="Z4" s="78"/>
+      <c r="AA4" s="78"/>
+      <c r="AB4" s="80"/>
+      <c r="AC4" s="71"/>
+      <c r="AD4" s="71"/>
+      <c r="AE4" s="71"/>
+      <c r="AF4" s="71"/>
+      <c r="AG4" s="71"/>
+      <c r="AH4" s="71"/>
+      <c r="AI4" s="71"/>
+      <c r="AJ4" s="71"/>
+      <c r="AK4" s="71"/>
+      <c r="AL4" s="71"/>
+      <c r="AM4" s="71"/>
+      <c r="AN4" s="71"/>
     </row>
     <row r="5" spans="1:40" ht="10" customHeight="1">
-      <c r="A5" s="117"/>
-      <c r="B5" s="72"/>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="82"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="82"/>
-      <c r="K5" s="82"/>
-      <c r="L5" s="82"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="82"/>
-      <c r="O5" s="72"/>
-      <c r="P5" s="82"/>
-      <c r="Q5" s="82"/>
-      <c r="R5" s="82"/>
-      <c r="S5" s="72"/>
-      <c r="T5" s="82"/>
-      <c r="U5" s="82"/>
-      <c r="V5" s="72"/>
-      <c r="W5" s="82"/>
-      <c r="X5" s="82"/>
-      <c r="Y5" s="72"/>
-      <c r="Z5" s="82"/>
-      <c r="AA5" s="82"/>
-      <c r="AB5" s="74"/>
-      <c r="AC5" s="72"/>
-      <c r="AD5" s="72"/>
-      <c r="AE5" s="72"/>
-      <c r="AF5" s="72"/>
-      <c r="AG5" s="72"/>
-      <c r="AH5" s="72"/>
-      <c r="AI5" s="72"/>
-      <c r="AJ5" s="72"/>
-      <c r="AK5" s="72"/>
-      <c r="AL5" s="72"/>
-      <c r="AM5" s="72"/>
-      <c r="AN5" s="72"/>
+      <c r="A5" s="94"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="81"/>
+      <c r="K5" s="81"/>
+      <c r="L5" s="81"/>
+      <c r="M5" s="71"/>
+      <c r="N5" s="81"/>
+      <c r="O5" s="71"/>
+      <c r="P5" s="81"/>
+      <c r="Q5" s="81"/>
+      <c r="R5" s="81"/>
+      <c r="S5" s="71"/>
+      <c r="T5" s="81"/>
+      <c r="U5" s="81"/>
+      <c r="V5" s="71"/>
+      <c r="W5" s="81"/>
+      <c r="X5" s="81"/>
+      <c r="Y5" s="71"/>
+      <c r="Z5" s="81"/>
+      <c r="AA5" s="81"/>
+      <c r="AB5" s="73"/>
+      <c r="AC5" s="71"/>
+      <c r="AD5" s="71"/>
+      <c r="AE5" s="71"/>
+      <c r="AF5" s="71"/>
+      <c r="AG5" s="71"/>
+      <c r="AH5" s="71"/>
+      <c r="AI5" s="71"/>
+      <c r="AJ5" s="71"/>
+      <c r="AK5" s="71"/>
+      <c r="AL5" s="71"/>
+      <c r="AM5" s="71"/>
+      <c r="AN5" s="71"/>
     </row>
     <row r="6" spans="1:40" ht="20" customHeight="1">
-      <c r="A6" s="121" t="s">
+      <c r="A6" s="99" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="109" t="s">
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="123" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="110"/>
-      <c r="G6" s="110"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="108" t="s">
+      <c r="F6" s="124"/>
+      <c r="G6" s="124"/>
+      <c r="H6" s="91"/>
+      <c r="I6" s="91"/>
+      <c r="J6" s="122" t="s">
         <v>47</v>
       </c>
-      <c r="K6" s="108"/>
-      <c r="L6" s="108"/>
-      <c r="M6" s="108"/>
-      <c r="N6" s="108"/>
-      <c r="O6" s="108"/>
-      <c r="P6" s="108"/>
-      <c r="Q6" s="108"/>
-      <c r="R6" s="108"/>
-      <c r="S6" s="108"/>
-      <c r="T6" s="92"/>
-      <c r="W6" s="109" t="s">
+      <c r="K6" s="122"/>
+      <c r="L6" s="122"/>
+      <c r="M6" s="122"/>
+      <c r="N6" s="122"/>
+      <c r="O6" s="122"/>
+      <c r="P6" s="122"/>
+      <c r="Q6" s="122"/>
+      <c r="R6" s="122"/>
+      <c r="S6" s="122"/>
+      <c r="T6" s="91"/>
+      <c r="W6" s="123" t="s">
         <v>48</v>
       </c>
-      <c r="X6" s="109"/>
-      <c r="Y6" s="109"/>
-      <c r="Z6" s="109"/>
-      <c r="AA6" s="109"/>
-      <c r="AB6" s="72"/>
-      <c r="AC6" s="72"/>
-      <c r="AD6" s="72"/>
-      <c r="AE6" s="72"/>
-      <c r="AF6" s="72"/>
-      <c r="AG6" s="72"/>
-      <c r="AH6" s="72"/>
-      <c r="AI6" s="72"/>
+      <c r="X6" s="123"/>
+      <c r="Y6" s="123"/>
+      <c r="Z6" s="123"/>
+      <c r="AA6" s="123"/>
+      <c r="AB6" s="71"/>
+      <c r="AC6" s="71"/>
+      <c r="AD6" s="71"/>
+      <c r="AE6" s="71"/>
+      <c r="AF6" s="71"/>
+      <c r="AG6" s="71"/>
+      <c r="AH6" s="71"/>
+      <c r="AI6" s="71"/>
     </row>
     <row r="7" spans="1:40" ht="10" customHeight="1">
-      <c r="A7" s="117"/>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="110"/>
-      <c r="F7" s="110"/>
-      <c r="G7" s="110"/>
-      <c r="H7" s="92"/>
-      <c r="I7" s="92"/>
-      <c r="J7" s="108"/>
-      <c r="K7" s="108"/>
-      <c r="L7" s="108"/>
-      <c r="M7" s="108"/>
-      <c r="N7" s="108"/>
-      <c r="O7" s="108"/>
-      <c r="P7" s="108"/>
-      <c r="Q7" s="108"/>
-      <c r="R7" s="108"/>
-      <c r="S7" s="108"/>
-      <c r="T7" s="92"/>
-      <c r="W7" s="109"/>
-      <c r="X7" s="109"/>
-      <c r="Y7" s="109"/>
-      <c r="Z7" s="109"/>
-      <c r="AA7" s="109"/>
-      <c r="AB7" s="72"/>
-      <c r="AC7" s="72"/>
-      <c r="AD7" s="72"/>
-      <c r="AE7" s="72"/>
-      <c r="AF7" s="72"/>
-      <c r="AG7" s="72"/>
-      <c r="AH7" s="72"/>
-      <c r="AI7" s="72"/>
+      <c r="A7" s="94"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="124"/>
+      <c r="F7" s="124"/>
+      <c r="G7" s="124"/>
+      <c r="H7" s="91"/>
+      <c r="I7" s="91"/>
+      <c r="J7" s="122"/>
+      <c r="K7" s="122"/>
+      <c r="L7" s="122"/>
+      <c r="M7" s="122"/>
+      <c r="N7" s="122"/>
+      <c r="O7" s="122"/>
+      <c r="P7" s="122"/>
+      <c r="Q7" s="122"/>
+      <c r="R7" s="122"/>
+      <c r="S7" s="122"/>
+      <c r="T7" s="91"/>
+      <c r="W7" s="123"/>
+      <c r="X7" s="123"/>
+      <c r="Y7" s="123"/>
+      <c r="Z7" s="123"/>
+      <c r="AA7" s="123"/>
+      <c r="AB7" s="71"/>
+      <c r="AC7" s="71"/>
+      <c r="AD7" s="71"/>
+      <c r="AE7" s="71"/>
+      <c r="AF7" s="71"/>
+      <c r="AG7" s="71"/>
+      <c r="AH7" s="71"/>
+      <c r="AI7" s="71"/>
     </row>
     <row r="8" spans="1:40" ht="26.25" customHeight="1">
-      <c r="A8" s="122"/>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="72"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="72"/>
-      <c r="L8" s="72"/>
-      <c r="M8" s="72"/>
-      <c r="N8" s="72"/>
-      <c r="O8" s="72"/>
-      <c r="P8" s="72"/>
-      <c r="Q8" s="72"/>
-      <c r="R8" s="72"/>
-      <c r="S8" s="72"/>
-      <c r="T8" s="72"/>
-      <c r="U8" s="72"/>
-      <c r="V8" s="72"/>
-      <c r="W8" s="72"/>
-      <c r="X8" s="72"/>
-      <c r="Y8" s="72"/>
-      <c r="Z8" s="72"/>
-      <c r="AA8" s="72"/>
-      <c r="AB8" s="72"/>
-      <c r="AC8" s="72"/>
-      <c r="AD8" s="72"/>
-      <c r="AE8" s="72"/>
-      <c r="AF8" s="72"/>
-      <c r="AG8" s="72"/>
-      <c r="AH8" s="72"/>
-      <c r="AI8" s="72"/>
-      <c r="AJ8" s="72"/>
-      <c r="AK8" s="72"/>
-      <c r="AL8" s="72"/>
-      <c r="AM8" s="72"/>
-      <c r="AN8" s="72"/>
+      <c r="A8" s="100"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="71"/>
+      <c r="J8" s="71"/>
+      <c r="K8" s="71"/>
+      <c r="L8" s="71"/>
+      <c r="M8" s="71"/>
+      <c r="N8" s="71"/>
+      <c r="O8" s="71"/>
+      <c r="P8" s="71"/>
+      <c r="Q8" s="71"/>
+      <c r="R8" s="71"/>
+      <c r="S8" s="71"/>
+      <c r="T8" s="71"/>
+      <c r="U8" s="71"/>
+      <c r="V8" s="71"/>
+      <c r="W8" s="71"/>
+      <c r="X8" s="71"/>
+      <c r="Y8" s="71"/>
+      <c r="Z8" s="71"/>
+      <c r="AA8" s="71"/>
+      <c r="AB8" s="71"/>
+      <c r="AC8" s="71"/>
+      <c r="AD8" s="71"/>
+      <c r="AE8" s="71"/>
+      <c r="AF8" s="71"/>
+      <c r="AG8" s="71"/>
+      <c r="AH8" s="71"/>
+      <c r="AI8" s="71"/>
+      <c r="AJ8" s="71"/>
+      <c r="AK8" s="71"/>
+      <c r="AL8" s="71"/>
+      <c r="AM8" s="71"/>
+      <c r="AN8" s="71"/>
     </row>
     <row r="9" spans="1:40" ht="10" customHeight="1">
-      <c r="A9" s="117"/>
-      <c r="B9" s="72"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="72"/>
-      <c r="J9" s="72"/>
-      <c r="K9" s="72"/>
-      <c r="L9" s="72"/>
-      <c r="M9" s="72"/>
-      <c r="N9" s="75"/>
-      <c r="O9" s="72"/>
-      <c r="P9" s="72"/>
-      <c r="Q9" s="72"/>
-      <c r="R9" s="72"/>
-      <c r="S9" s="72"/>
-      <c r="T9" s="72"/>
-      <c r="U9" s="72"/>
-      <c r="V9" s="72"/>
-      <c r="W9" s="72"/>
-      <c r="X9" s="72"/>
-      <c r="Y9" s="72"/>
-      <c r="Z9" s="75"/>
-      <c r="AA9" s="75"/>
-      <c r="AB9" s="74"/>
-      <c r="AC9" s="72"/>
-      <c r="AD9" s="72"/>
-      <c r="AE9" s="72"/>
-      <c r="AF9" s="72"/>
-      <c r="AG9" s="72"/>
-      <c r="AH9" s="72"/>
-      <c r="AI9" s="72"/>
-      <c r="AJ9" s="72"/>
-      <c r="AK9" s="72"/>
-      <c r="AL9" s="72"/>
-      <c r="AM9" s="72"/>
-      <c r="AN9" s="72"/>
+      <c r="A9" s="94"/>
+      <c r="B9" s="71"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="71"/>
+      <c r="K9" s="71"/>
+      <c r="L9" s="71"/>
+      <c r="M9" s="71"/>
+      <c r="N9" s="74"/>
+      <c r="O9" s="71"/>
+      <c r="P9" s="71"/>
+      <c r="Q9" s="71"/>
+      <c r="R9" s="71"/>
+      <c r="S9" s="71"/>
+      <c r="T9" s="71"/>
+      <c r="U9" s="71"/>
+      <c r="V9" s="71"/>
+      <c r="W9" s="71"/>
+      <c r="X9" s="71"/>
+      <c r="Y9" s="71"/>
+      <c r="Z9" s="74"/>
+      <c r="AA9" s="74"/>
+      <c r="AB9" s="73"/>
+      <c r="AC9" s="71"/>
+      <c r="AD9" s="71"/>
+      <c r="AE9" s="71"/>
+      <c r="AF9" s="71"/>
+      <c r="AG9" s="71"/>
+      <c r="AH9" s="71"/>
+      <c r="AI9" s="71"/>
+      <c r="AJ9" s="71"/>
+      <c r="AK9" s="71"/>
+      <c r="AL9" s="71"/>
+      <c r="AM9" s="71"/>
+      <c r="AN9" s="71"/>
     </row>
     <row r="10" spans="1:40" ht="35" customHeight="1">
-      <c r="A10" s="119" t="s">
+      <c r="A10" s="97" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="72"/>
-      <c r="C10" s="83"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="85"/>
-      <c r="F10" s="85"/>
-      <c r="G10" s="76"/>
-      <c r="H10" s="79"/>
-      <c r="I10" s="86"/>
-      <c r="J10" s="83"/>
-      <c r="K10" s="85"/>
-      <c r="L10" s="85"/>
-      <c r="M10" s="76"/>
-      <c r="N10" s="79"/>
-      <c r="O10" s="86"/>
-      <c r="P10" s="83"/>
-      <c r="Q10" s="84"/>
-      <c r="R10" s="85"/>
-      <c r="S10" s="72"/>
-      <c r="T10" s="79"/>
-      <c r="U10" s="79"/>
-      <c r="V10" s="72"/>
-      <c r="W10" s="84"/>
-      <c r="X10" s="85"/>
-      <c r="Y10" s="87"/>
-      <c r="Z10" s="79"/>
-      <c r="AA10" s="79"/>
-      <c r="AB10" s="81"/>
-      <c r="AC10" s="72"/>
-      <c r="AD10" s="72"/>
-      <c r="AE10" s="72"/>
-      <c r="AF10" s="72"/>
-      <c r="AG10" s="72"/>
-      <c r="AH10" s="72"/>
-      <c r="AI10" s="72"/>
-      <c r="AJ10" s="72"/>
-      <c r="AK10" s="72"/>
-      <c r="AL10" s="72"/>
-      <c r="AM10" s="72"/>
-      <c r="AN10" s="72"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="83"/>
+      <c r="E10" s="84"/>
+      <c r="F10" s="84"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="78"/>
+      <c r="I10" s="85"/>
+      <c r="J10" s="82"/>
+      <c r="K10" s="84"/>
+      <c r="L10" s="84"/>
+      <c r="M10" s="75"/>
+      <c r="N10" s="78"/>
+      <c r="O10" s="85"/>
+      <c r="P10" s="82"/>
+      <c r="Q10" s="83"/>
+      <c r="R10" s="84"/>
+      <c r="S10" s="71"/>
+      <c r="T10" s="78"/>
+      <c r="U10" s="78"/>
+      <c r="V10" s="71"/>
+      <c r="W10" s="83"/>
+      <c r="X10" s="84"/>
+      <c r="Y10" s="86"/>
+      <c r="Z10" s="78"/>
+      <c r="AA10" s="78"/>
+      <c r="AB10" s="80"/>
+      <c r="AC10" s="71"/>
+      <c r="AD10" s="71"/>
+      <c r="AE10" s="71"/>
+      <c r="AF10" s="71"/>
+      <c r="AG10" s="71"/>
+      <c r="AH10" s="71"/>
+      <c r="AI10" s="71"/>
+      <c r="AJ10" s="71"/>
+      <c r="AK10" s="71"/>
+      <c r="AL10" s="71"/>
+      <c r="AM10" s="71"/>
+      <c r="AN10" s="71"/>
     </row>
     <row r="11" spans="1:40" ht="10" customHeight="1">
-      <c r="A11" s="120"/>
-      <c r="B11" s="74"/>
-      <c r="C11" s="74"/>
-      <c r="D11" s="74"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74"/>
-      <c r="H11" s="88"/>
-      <c r="I11" s="72"/>
-      <c r="J11" s="74"/>
-      <c r="K11" s="74"/>
-      <c r="L11" s="74"/>
-      <c r="M11" s="72"/>
-      <c r="N11" s="88"/>
-      <c r="O11" s="72"/>
-      <c r="P11" s="74"/>
-      <c r="Q11" s="74"/>
-      <c r="R11" s="74"/>
-      <c r="S11" s="72"/>
-      <c r="T11" s="74"/>
-      <c r="U11" s="74"/>
-      <c r="V11" s="72"/>
-      <c r="W11" s="74"/>
-      <c r="X11" s="74"/>
-      <c r="Y11" s="74"/>
-      <c r="Z11" s="88"/>
-      <c r="AA11" s="88"/>
-      <c r="AB11" s="74"/>
-      <c r="AC11" s="74"/>
-      <c r="AD11" s="74"/>
-      <c r="AE11" s="74"/>
-      <c r="AF11" s="74"/>
-      <c r="AG11" s="74"/>
-      <c r="AH11" s="74"/>
-      <c r="AI11" s="74"/>
-      <c r="AJ11" s="74"/>
-      <c r="AK11" s="74"/>
-      <c r="AL11" s="74"/>
-      <c r="AM11" s="74"/>
-      <c r="AN11" s="74"/>
+      <c r="A11" s="98"/>
+      <c r="B11" s="73"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="73"/>
+      <c r="G11" s="73"/>
+      <c r="H11" s="87"/>
+      <c r="I11" s="71"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="73"/>
+      <c r="M11" s="71"/>
+      <c r="N11" s="87"/>
+      <c r="O11" s="71"/>
+      <c r="P11" s="73"/>
+      <c r="Q11" s="73"/>
+      <c r="R11" s="73"/>
+      <c r="S11" s="71"/>
+      <c r="T11" s="73"/>
+      <c r="U11" s="73"/>
+      <c r="V11" s="71"/>
+      <c r="W11" s="73"/>
+      <c r="X11" s="73"/>
+      <c r="Y11" s="73"/>
+      <c r="Z11" s="87"/>
+      <c r="AA11" s="87"/>
+      <c r="AB11" s="73"/>
+      <c r="AC11" s="73"/>
+      <c r="AD11" s="73"/>
+      <c r="AE11" s="73"/>
+      <c r="AF11" s="73"/>
+      <c r="AG11" s="73"/>
+      <c r="AH11" s="73"/>
+      <c r="AI11" s="73"/>
+      <c r="AJ11" s="73"/>
+      <c r="AK11" s="73"/>
+      <c r="AL11" s="73"/>
+      <c r="AM11" s="73"/>
+      <c r="AN11" s="73"/>
     </row>
     <row r="12" spans="1:40" ht="20" customHeight="1">
-      <c r="A12" s="121" t="s">
+      <c r="A12" s="99" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="74"/>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="108" t="s">
+      <c r="B12" s="73"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="122" t="s">
         <v>44</v>
       </c>
-      <c r="G12" s="108"/>
-      <c r="H12" s="108"/>
-      <c r="I12" s="108"/>
-      <c r="J12" s="108"/>
-      <c r="K12" s="92"/>
-      <c r="L12" s="92"/>
-      <c r="M12" s="93"/>
-      <c r="P12" s="108" t="s">
+      <c r="G12" s="122"/>
+      <c r="H12" s="122"/>
+      <c r="I12" s="122"/>
+      <c r="J12" s="122"/>
+      <c r="K12" s="91"/>
+      <c r="L12" s="91"/>
+      <c r="M12" s="92"/>
+      <c r="P12" s="122" t="s">
         <v>45</v>
       </c>
-      <c r="Q12" s="108"/>
-      <c r="R12" s="108"/>
-      <c r="S12" s="108"/>
-      <c r="T12" s="108"/>
-      <c r="U12" s="108"/>
-      <c r="V12" s="108"/>
-      <c r="W12" s="108"/>
-      <c r="X12" s="108"/>
-      <c r="Y12" s="74"/>
-      <c r="Z12" s="74"/>
-      <c r="AA12" s="74"/>
-      <c r="AB12" s="74"/>
-      <c r="AC12" s="74"/>
+      <c r="Q12" s="122"/>
+      <c r="R12" s="122"/>
+      <c r="S12" s="122"/>
+      <c r="T12" s="122"/>
+      <c r="U12" s="122"/>
+      <c r="V12" s="122"/>
+      <c r="W12" s="122"/>
+      <c r="X12" s="122"/>
+      <c r="Y12" s="73"/>
+      <c r="Z12" s="73"/>
+      <c r="AA12" s="73"/>
+      <c r="AB12" s="73"/>
+      <c r="AC12" s="73"/>
     </row>
     <row r="13" spans="1:40" ht="10" customHeight="1">
-      <c r="A13" s="120"/>
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="74"/>
-      <c r="H13" s="74"/>
-      <c r="I13" s="72"/>
-      <c r="J13" s="74"/>
-      <c r="K13" s="74"/>
-      <c r="L13" s="74"/>
-      <c r="M13" s="72"/>
-      <c r="N13" s="74"/>
-      <c r="O13" s="72"/>
-      <c r="P13" s="74"/>
-      <c r="Q13" s="74"/>
-      <c r="R13" s="74"/>
-      <c r="S13" s="72"/>
-      <c r="T13" s="74"/>
-      <c r="U13" s="74"/>
-      <c r="V13" s="72"/>
-      <c r="W13" s="74"/>
-      <c r="X13" s="74"/>
-      <c r="Y13" s="74"/>
-      <c r="Z13" s="74"/>
-      <c r="AA13" s="74"/>
-      <c r="AB13" s="74"/>
-      <c r="AC13" s="74"/>
-      <c r="AD13" s="89"/>
-      <c r="AE13" s="89"/>
-      <c r="AF13" s="89"/>
-      <c r="AG13" s="89"/>
-      <c r="AH13" s="89"/>
-      <c r="AI13" s="89"/>
-      <c r="AJ13" s="74"/>
-      <c r="AK13" s="74"/>
-      <c r="AL13" s="74"/>
-      <c r="AM13" s="74"/>
-      <c r="AN13" s="74"/>
+      <c r="A13" s="98"/>
+      <c r="B13" s="73"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="71"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="73"/>
+      <c r="L13" s="73"/>
+      <c r="M13" s="71"/>
+      <c r="N13" s="73"/>
+      <c r="O13" s="71"/>
+      <c r="P13" s="73"/>
+      <c r="Q13" s="73"/>
+      <c r="R13" s="73"/>
+      <c r="S13" s="71"/>
+      <c r="T13" s="73"/>
+      <c r="U13" s="73"/>
+      <c r="V13" s="71"/>
+      <c r="W13" s="73"/>
+      <c r="X13" s="73"/>
+      <c r="Y13" s="73"/>
+      <c r="Z13" s="73"/>
+      <c r="AA13" s="73"/>
+      <c r="AB13" s="73"/>
+      <c r="AC13" s="73"/>
+      <c r="AD13" s="88"/>
+      <c r="AE13" s="88"/>
+      <c r="AF13" s="88"/>
+      <c r="AG13" s="88"/>
+      <c r="AH13" s="88"/>
+      <c r="AI13" s="88"/>
+      <c r="AJ13" s="73"/>
+      <c r="AK13" s="73"/>
+      <c r="AL13" s="73"/>
+      <c r="AM13" s="73"/>
+      <c r="AN13" s="73"/>
     </row>
     <row r="14" spans="1:40" ht="35" customHeight="1">
-      <c r="A14" s="119" t="s">
+      <c r="A14" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="72"/>
-      <c r="H14" s="72"/>
-      <c r="I14" s="72"/>
-      <c r="J14" s="72"/>
-      <c r="K14" s="72"/>
-      <c r="L14" s="72"/>
-      <c r="M14" s="72"/>
-      <c r="N14" s="72"/>
-      <c r="O14" s="72"/>
-      <c r="P14" s="72"/>
-      <c r="Q14" s="72"/>
-      <c r="R14" s="72"/>
-      <c r="S14" s="72"/>
-      <c r="T14" s="72"/>
-      <c r="U14" s="72"/>
-      <c r="V14" s="72"/>
-      <c r="W14" s="72"/>
-      <c r="X14" s="72"/>
-      <c r="Y14" s="72"/>
-      <c r="Z14" s="72"/>
-      <c r="AA14" s="72"/>
-      <c r="AB14" s="74"/>
-      <c r="AC14" s="76"/>
-      <c r="AD14" s="90"/>
-      <c r="AE14" s="90"/>
-      <c r="AF14" s="90"/>
-      <c r="AG14" s="90"/>
-      <c r="AH14" s="90"/>
-      <c r="AI14" s="90"/>
-      <c r="AJ14" s="86"/>
-      <c r="AK14" s="72"/>
-      <c r="AL14" s="72"/>
-      <c r="AM14" s="72"/>
-      <c r="AN14" s="72"/>
+      <c r="B14" s="71"/>
+      <c r="C14" s="71"/>
+      <c r="D14" s="71"/>
+      <c r="E14" s="71"/>
+      <c r="F14" s="71"/>
+      <c r="G14" s="71"/>
+      <c r="H14" s="71"/>
+      <c r="I14" s="71"/>
+      <c r="J14" s="71"/>
+      <c r="K14" s="71"/>
+      <c r="L14" s="71"/>
+      <c r="M14" s="71"/>
+      <c r="N14" s="71"/>
+      <c r="O14" s="71"/>
+      <c r="P14" s="71"/>
+      <c r="Q14" s="71"/>
+      <c r="R14" s="71"/>
+      <c r="S14" s="71"/>
+      <c r="T14" s="71"/>
+      <c r="U14" s="71"/>
+      <c r="V14" s="71"/>
+      <c r="W14" s="71"/>
+      <c r="X14" s="71"/>
+      <c r="Y14" s="71"/>
+      <c r="Z14" s="71"/>
+      <c r="AA14" s="71"/>
+      <c r="AB14" s="73"/>
+      <c r="AC14" s="75"/>
+      <c r="AD14" s="89"/>
+      <c r="AE14" s="89"/>
+      <c r="AF14" s="89"/>
+      <c r="AG14" s="89"/>
+      <c r="AH14" s="89"/>
+      <c r="AI14" s="89"/>
+      <c r="AJ14" s="85"/>
+      <c r="AK14" s="71"/>
+      <c r="AL14" s="71"/>
+      <c r="AM14" s="71"/>
+      <c r="AN14" s="71"/>
     </row>
     <row r="15" spans="1:40" ht="10" customHeight="1">
-      <c r="A15" s="120"/>
-      <c r="B15" s="72"/>
-      <c r="C15" s="72"/>
-      <c r="D15" s="72"/>
-      <c r="E15" s="72"/>
-      <c r="F15" s="72"/>
-      <c r="G15" s="72"/>
-      <c r="H15" s="72"/>
-      <c r="I15" s="72"/>
-      <c r="J15" s="72"/>
-      <c r="K15" s="72"/>
-      <c r="L15" s="72"/>
-      <c r="M15" s="72"/>
-      <c r="N15" s="72"/>
-      <c r="O15" s="72"/>
-      <c r="P15" s="72"/>
-      <c r="Q15" s="72"/>
-      <c r="R15" s="72"/>
-      <c r="S15" s="72"/>
-      <c r="T15" s="72"/>
-      <c r="U15" s="72"/>
-      <c r="V15" s="72"/>
-      <c r="W15" s="72"/>
-      <c r="X15" s="91"/>
-      <c r="Y15" s="72"/>
-      <c r="Z15" s="72"/>
-      <c r="AA15" s="72"/>
-      <c r="AB15" s="74"/>
-      <c r="AC15" s="72"/>
-      <c r="AD15" s="82"/>
-      <c r="AE15" s="82"/>
-      <c r="AF15" s="82"/>
-      <c r="AG15" s="82"/>
-      <c r="AH15" s="82"/>
-      <c r="AI15" s="82"/>
-      <c r="AJ15" s="72"/>
-      <c r="AK15" s="72"/>
-      <c r="AL15" s="72"/>
-      <c r="AM15" s="72"/>
-      <c r="AN15" s="72"/>
+      <c r="A15" s="98"/>
+      <c r="B15" s="71"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="71"/>
+      <c r="F15" s="71"/>
+      <c r="G15" s="71"/>
+      <c r="H15" s="71"/>
+      <c r="I15" s="71"/>
+      <c r="J15" s="71"/>
+      <c r="K15" s="71"/>
+      <c r="L15" s="71"/>
+      <c r="M15" s="71"/>
+      <c r="N15" s="71"/>
+      <c r="O15" s="71"/>
+      <c r="P15" s="71"/>
+      <c r="Q15" s="71"/>
+      <c r="R15" s="71"/>
+      <c r="S15" s="71"/>
+      <c r="T15" s="71"/>
+      <c r="U15" s="71"/>
+      <c r="V15" s="71"/>
+      <c r="W15" s="71"/>
+      <c r="X15" s="90"/>
+      <c r="Y15" s="71"/>
+      <c r="Z15" s="71"/>
+      <c r="AA15" s="71"/>
+      <c r="AB15" s="73"/>
+      <c r="AC15" s="71"/>
+      <c r="AD15" s="81"/>
+      <c r="AE15" s="81"/>
+      <c r="AF15" s="81"/>
+      <c r="AG15" s="81"/>
+      <c r="AH15" s="81"/>
+      <c r="AI15" s="81"/>
+      <c r="AJ15" s="71"/>
+      <c r="AK15" s="71"/>
+      <c r="AL15" s="71"/>
+      <c r="AM15" s="71"/>
+      <c r="AN15" s="71"/>
     </row>
     <row r="16" spans="1:40" ht="20" customHeight="1">
-      <c r="A16" s="121" t="s">
+      <c r="A16" s="99" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="72"/>
-      <c r="C16" s="72"/>
-      <c r="D16" s="72"/>
-      <c r="E16" s="72"/>
-      <c r="F16" s="72"/>
-      <c r="G16" s="72"/>
-      <c r="H16" s="72"/>
-      <c r="I16" s="72"/>
-      <c r="J16" s="72"/>
-      <c r="K16" s="72"/>
-      <c r="L16" s="72"/>
-      <c r="M16" s="72"/>
-      <c r="N16" s="72"/>
-      <c r="O16" s="72"/>
-      <c r="P16" s="72"/>
-      <c r="Q16" s="72"/>
-      <c r="R16" s="72"/>
-      <c r="S16" s="72"/>
-      <c r="T16" s="72"/>
-      <c r="U16" s="72"/>
-      <c r="V16" s="72"/>
-      <c r="W16" s="72"/>
-      <c r="X16" s="72"/>
-      <c r="Y16" s="72"/>
-      <c r="Z16" s="72"/>
-      <c r="AA16" s="72"/>
-      <c r="AB16" s="74"/>
-      <c r="AC16" s="72"/>
-      <c r="AD16" s="72"/>
-      <c r="AE16" s="72"/>
-      <c r="AF16" s="72"/>
-      <c r="AG16" s="72"/>
-      <c r="AH16" s="72"/>
-      <c r="AI16" s="108" t="s">
+      <c r="B16" s="71"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="71"/>
+      <c r="F16" s="71"/>
+      <c r="G16" s="71"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="71"/>
+      <c r="J16" s="71"/>
+      <c r="K16" s="71"/>
+      <c r="L16" s="71"/>
+      <c r="M16" s="71"/>
+      <c r="N16" s="71"/>
+      <c r="O16" s="71"/>
+      <c r="P16" s="71"/>
+      <c r="Q16" s="71"/>
+      <c r="R16" s="71"/>
+      <c r="S16" s="71"/>
+      <c r="T16" s="71"/>
+      <c r="U16" s="71"/>
+      <c r="V16" s="71"/>
+      <c r="W16" s="71"/>
+      <c r="X16" s="71"/>
+      <c r="Y16" s="71"/>
+      <c r="Z16" s="71"/>
+      <c r="AA16" s="71"/>
+      <c r="AB16" s="73"/>
+      <c r="AC16" s="71"/>
+      <c r="AD16" s="71"/>
+      <c r="AE16" s="71"/>
+      <c r="AF16" s="71"/>
+      <c r="AG16" s="71"/>
+      <c r="AH16" s="71"/>
+      <c r="AI16" s="122" t="s">
         <v>43</v>
       </c>
-      <c r="AJ16" s="108"/>
-      <c r="AK16" s="108"/>
-      <c r="AL16" s="108"/>
-      <c r="AM16" s="108"/>
-      <c r="AN16" s="72"/>
+      <c r="AJ16" s="122"/>
+      <c r="AK16" s="122"/>
+      <c r="AL16" s="122"/>
+      <c r="AM16" s="122"/>
+      <c r="AN16" s="71"/>
     </row>
     <row r="17" spans="1:40" ht="10" customHeight="1">
-      <c r="A17" s="74"/>
-      <c r="B17" s="72"/>
-      <c r="C17" s="72"/>
-      <c r="D17" s="72"/>
-      <c r="E17" s="72"/>
-      <c r="F17" s="72"/>
-      <c r="G17" s="72"/>
-      <c r="H17" s="72"/>
-      <c r="I17" s="72"/>
-      <c r="J17" s="72"/>
-      <c r="K17" s="72"/>
-      <c r="L17" s="72"/>
-      <c r="M17" s="72"/>
-      <c r="N17" s="72"/>
-      <c r="O17" s="72"/>
-      <c r="P17" s="72"/>
-      <c r="Q17" s="72"/>
-      <c r="R17" s="72"/>
-      <c r="S17" s="72"/>
-      <c r="T17" s="72"/>
-      <c r="U17" s="72"/>
-      <c r="V17" s="72"/>
-      <c r="W17" s="72"/>
-      <c r="X17" s="72"/>
-      <c r="Y17" s="72"/>
-      <c r="Z17" s="72"/>
-      <c r="AA17" s="72"/>
-      <c r="AB17" s="74"/>
-      <c r="AC17" s="72"/>
-      <c r="AD17" s="72"/>
-      <c r="AE17" s="72"/>
-      <c r="AF17" s="72"/>
-      <c r="AG17" s="72"/>
-      <c r="AH17" s="72"/>
-      <c r="AI17" s="72"/>
-      <c r="AJ17" s="72"/>
-      <c r="AK17" s="72"/>
-      <c r="AL17" s="72"/>
-      <c r="AM17" s="72"/>
-      <c r="AN17" s="72"/>
+      <c r="A17" s="73"/>
+      <c r="B17" s="71"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="71"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="71"/>
+      <c r="J17" s="71"/>
+      <c r="K17" s="71"/>
+      <c r="L17" s="71"/>
+      <c r="M17" s="71"/>
+      <c r="N17" s="71"/>
+      <c r="O17" s="71"/>
+      <c r="P17" s="71"/>
+      <c r="Q17" s="71"/>
+      <c r="R17" s="71"/>
+      <c r="S17" s="71"/>
+      <c r="T17" s="71"/>
+      <c r="U17" s="71"/>
+      <c r="V17" s="71"/>
+      <c r="W17" s="71"/>
+      <c r="X17" s="71"/>
+      <c r="Y17" s="71"/>
+      <c r="Z17" s="71"/>
+      <c r="AA17" s="71"/>
+      <c r="AB17" s="73"/>
+      <c r="AC17" s="71"/>
+      <c r="AD17" s="71"/>
+      <c r="AE17" s="71"/>
+      <c r="AF17" s="71"/>
+      <c r="AG17" s="71"/>
+      <c r="AH17" s="71"/>
+      <c r="AI17" s="71"/>
+      <c r="AJ17" s="71"/>
+      <c r="AK17" s="71"/>
+      <c r="AL17" s="71"/>
+      <c r="AM17" s="71"/>
+      <c r="AN17" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="F12:J12"/>
+    <mergeCell ref="P12:X12"/>
+    <mergeCell ref="AI16:AM16"/>
+    <mergeCell ref="E6:G7"/>
+    <mergeCell ref="J6:S7"/>
+    <mergeCell ref="W6:AA7"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:J1"/>
     <mergeCell ref="K1:P1"/>
@@ -6558,12 +6564,6 @@
     <mergeCell ref="W1:Z1"/>
     <mergeCell ref="Q1:U1"/>
     <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="F12:J12"/>
-    <mergeCell ref="P12:X12"/>
-    <mergeCell ref="AI16:AM16"/>
-    <mergeCell ref="E6:G7"/>
-    <mergeCell ref="J6:S7"/>
-    <mergeCell ref="W6:AA7"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>